<commit_message>
Reduced the check frequency of the limit switches. Tried to implement a proportional controller but it didn't really work, so it's left commented out. Should tidy up code at some point and delete leftover variables.
</commit_message>
<xml_diff>
--- a/GantryControl_v0.5/Step Size Calculator.xlsx
+++ b/GantryControl_v0.5/Step Size Calculator.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Step size</t>
   </si>
@@ -63,6 +63,21 @@
   </si>
   <si>
     <t>Calculator</t>
+  </si>
+  <si>
+    <t>Conversion</t>
+  </si>
+  <si>
+    <t>Equivalent Steps</t>
+  </si>
+  <si>
+    <t>X Offset</t>
+  </si>
+  <si>
+    <t>Y Offset</t>
+  </si>
+  <si>
+    <t>Boundary Offset</t>
   </si>
 </sst>
 </file>
@@ -450,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:F11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,20 +477,23 @@
     <col min="5" max="5" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="1">
-        <v>0.15</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -484,13 +502,17 @@
         <v>9</v>
       </c>
       <c r="F2">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="G2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <f>ROUND(F2*$B$7,0)</f>
+        <v>637</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -504,13 +526,17 @@
         <v>10</v>
       </c>
       <c r="F3">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="G3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H7" si="0">ROUND(F3*$B$7,0)</f>
+        <v>573</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -529,22 +555,76 @@
       <c r="G4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>4934</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>0.05</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <f>360/(2*PI()*B3/100*B4*B5)</f>
+        <v>3183.0988618379065</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7">
+        <v>0.3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>955</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
-        <f>ROUND(B2*360/(2*PI()*B3/100*B4*B5),0)</f>
-        <v>477</v>
+      <c r="B8" s="2">
+        <f>ROUND(B7*B2,0)</f>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>